<commit_message>
Math and test libraries reworked
</commit_message>
<xml_diff>
--- a/Excel/ExcelAlgorithm.xlsx
+++ b/Excel/ExcelAlgorithm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RestaurantKursovaya\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RestaurantKursovaya\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD4E6-1382-48AE-AF90-296F85F00939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFA64F4-7923-456B-9961-8865A244F5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9DEF4581-84BC-4201-AE19-961D2FB44A1C}"/>
   </bookViews>
@@ -641,7 +641,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="P4">
         <f>SUMIFS(Больничные!J:J,Больничные!B:B,Сотрудники!$A4)</f>
-        <v>3207</v>
+        <v>3848.3999999999996</v>
       </c>
       <c r="Q4">
         <f>SUMIFS('Сверхурочные часы'!E:E,'Сверхурочные часы'!B:B,Сотрудники!$A4)</f>
@@ -909,7 +909,7 @@
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>20217</v>
+        <v>20858.400000000001</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1083,7 +1083,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34D3219-4CF5-47C6-B66E-3AAAE28E6D51}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1240,16 +1240,16 @@
         <v>3150</v>
       </c>
       <c r="H2" cm="1">
-        <f t="array" ref="H2">INDEX(Сотрудники!H:H,Больничные!B2+1)*INDEX(Сотрудники!K:K,Больничные!B2)</f>
-        <v>120</v>
+        <f t="array" ref="H2">INDEX(Сотрудники!H:H,Больничные!B2+1)*INDEX(Сотрудники!K:K,Больничные!B2+1)</f>
+        <v>100</v>
       </c>
       <c r="I2">
         <f>$L$2/H2</f>
-        <v>160.35</v>
+        <v>192.42</v>
       </c>
       <c r="J2">
         <f>I2*F2</f>
-        <v>2405.25</v>
+        <v>2886.2999999999997</v>
       </c>
       <c r="L2" s="3">
         <v>19242</v>
@@ -1277,16 +1277,16 @@
         <v>1050</v>
       </c>
       <c r="H3" cm="1">
-        <f t="array" ref="H3">INDEX(Сотрудники!H:H,Больничные!B3+1)*INDEX(Сотрудники!K:K,Больничные!B3)</f>
-        <v>120</v>
+        <f t="array" ref="H3">INDEX(Сотрудники!H:H,Больничные!B3+1)*INDEX(Сотрудники!K:K,Больничные!B3+1)</f>
+        <v>100</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I4" si="0">$L$2/H3</f>
-        <v>160.35</v>
+        <v>192.42</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J4" si="1">I3*F3</f>
-        <v>801.75</v>
+        <v>962.09999999999991</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1311,7 +1311,7 @@
         <v>2520</v>
       </c>
       <c r="H4" cm="1">
-        <f t="array" ref="H4">INDEX(Сотрудники!H:H,Больничные!B4+1)*INDEX(Сотрудники!K:K,Больничные!B4)</f>
+        <f t="array" ref="H4">INDEX(Сотрудники!H:H,Больничные!B4+1)*INDEX(Сотрудники!K:K,Больничные!B4+1)</f>
         <v>288</v>
       </c>
       <c r="I4">

</xml_diff>